<commit_message>
Updated input data files
Updated example models.
</commit_message>
<xml_diff>
--- a/input_data/demo_model.xlsx
+++ b/input_data/demo_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E67E9D-A21D-41F5-BCC2-3508307764D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419E621D-FB4C-4CA1-83B3-CC8D7801C6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="796" activeTab="6" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="126">
   <si>
     <t>node</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>initial_flow</t>
+  </si>
+  <si>
+    <t>node_dummy_variable_cost</t>
+  </si>
+  <si>
+    <t>ramp_dummy_variable_cost</t>
   </si>
 </sst>
 </file>
@@ -4955,178 +4961,178 @@
       <selection activeCell="A8" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
     </row>
   </sheetData>
@@ -5143,12 +5149,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -5173,9 +5179,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -5196,15 +5202,15 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="2" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="2" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5218,7 +5224,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5235,7 +5241,7 @@
       <c r="F2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5250,7 +5256,7 @@
         <v>0.34899999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5265,7 +5271,7 @@
         <v>0.27899999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5280,7 +5286,7 @@
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5295,7 +5301,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5310,7 +5316,7 @@
         <v>0.23500000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5325,7 +5331,7 @@
         <v>0.17500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5340,7 +5346,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5355,7 +5361,7 @@
         <v>0.21400000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5370,85 +5376,85 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -5470,14 +5476,14 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="4" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="4" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5491,7 +5497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5508,7 +5514,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5525,7 +5531,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5542,7 +5548,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5559,7 +5565,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5576,7 +5582,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5593,7 +5599,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5610,7 +5616,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5627,7 +5633,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5644,7 +5650,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5661,7 +5667,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
@@ -5669,7 +5675,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
@@ -5677,7 +5683,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
@@ -5685,7 +5691,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
@@ -5693,7 +5699,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
@@ -5701,7 +5707,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
@@ -5709,7 +5715,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
@@ -5717,7 +5723,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
@@ -5725,7 +5731,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
@@ -5733,7 +5739,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
@@ -5741,7 +5747,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
@@ -5749,7 +5755,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
@@ -5757,7 +5763,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
@@ -5765,7 +5771,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -5789,82 +5795,82 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="3" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -5883,12 +5889,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5896,7 +5902,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5905,7 +5911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5914,7 +5920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5923,7 +5929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5932,7 +5938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5941,7 +5947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5950,7 +5956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -5959,7 +5965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -5968,7 +5974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -5977,7 +5983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -5986,85 +5992,85 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -6084,19 +6090,19 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="2" max="2" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -6134,7 +6140,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -6172,13 +6178,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I5"/>
     </row>
   </sheetData>
@@ -6194,21 +6200,21 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
     </row>
   </sheetData>
@@ -6224,14 +6230,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="2" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="14" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="2" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="14" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -6245,7 +6251,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -6260,7 +6266,7 @@
         <v>8.98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -6275,7 +6281,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -6290,7 +6296,7 @@
         <v>25.19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -6305,7 +6311,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -6320,7 +6326,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -6335,7 +6341,7 @@
         <v>23.67</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -6350,7 +6356,7 @@
         <v>50.43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -6365,7 +6371,7 @@
         <v>36.69</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -6380,7 +6386,7 @@
         <v>6.36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -6411,15 +6417,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -6443,7 +6449,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -6473,7 +6479,7 @@
         <v>8.5310000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -6503,7 +6509,7 @@
         <v>4.2560000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -6533,7 +6539,7 @@
         <v>23.930499999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -6563,7 +6569,7 @@
         <v>18.145</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -6593,7 +6599,7 @@
         <v>24.519499999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -6623,7 +6629,7 @@
         <v>22.486499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -6653,7 +6659,7 @@
         <v>47.908499999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -6683,7 +6689,7 @@
         <v>34.855499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -6713,7 +6719,7 @@
         <v>6.0419999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -6743,10 +6749,10 @@
         <v>14.1455</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6754,40 +6760,40 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
     </row>
   </sheetData>
@@ -6798,19 +6804,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB98B755-8BE1-4837-9877-4DDB59C80C3F}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -6818,7 +6824,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -6826,7 +6832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -6834,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -6842,7 +6848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -6850,7 +6856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -6858,16 +6864,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>118</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -6885,12 +6907,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -6898,7 +6920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -6906,7 +6928,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -6927,9 +6949,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -6937,7 +6959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6945,7 +6967,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6953,7 +6975,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -6974,162 +6996,162 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -7148,155 +7170,155 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -7316,155 +7338,155 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -7483,14 +7505,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -7504,7 +7526,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -7518,7 +7540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -7535,17 +7557,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="2" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -7577,7 +7599,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -7610,7 +7632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -7643,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -7676,7 +7698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -7709,7 +7731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -7742,7 +7764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -7775,7 +7797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
@@ -7808,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
@@ -7841,7 +7863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
@@ -7874,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
@@ -7907,85 +7929,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -8004,20 +8026,20 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8067,7 +8089,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -8117,7 +8139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -8167,7 +8189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -8217,7 +8239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -8267,7 +8289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -8299,23 +8321,23 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -8368,7 +8390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -8421,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -8474,7 +8496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -8527,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -8580,7 +8602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -8646,9 +8668,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -8659,7 +8681,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8670,7 +8692,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -8681,7 +8703,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -8692,7 +8714,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -8703,7 +8725,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -8727,9 +8749,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -8782,24 +8804,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -8831,7 +8853,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -8863,7 +8885,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>65</v>
       </c>
@@ -8895,7 +8917,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
@@ -8927,7 +8949,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -8959,7 +8981,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -8991,7 +9013,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -9023,7 +9045,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -9055,7 +9077,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -9087,7 +9109,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
@@ -9119,7 +9141,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>91</v>
       </c>
@@ -9165,155 +9187,155 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999537038</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666087964</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332638889</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999189815</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -9332,14 +9354,14 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Updated example input data files
</commit_message>
<xml_diff>
--- a/input_data/demo_model.xlsx
+++ b/input_data/demo_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419E621D-FB4C-4CA1-83B3-CC8D7801C6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557D5659-7B2B-44ED-8FA5-9477E9380E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" firstSheet="10" activeTab="16" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="125">
   <si>
     <t>node</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>penalty</t>
-  </si>
-  <si>
-    <t>reserve_product</t>
   </si>
   <si>
     <t>processgroup</t>
@@ -488,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -502,9 +499,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5156,13 +5150,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5221,7 +5215,7 @@
         <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -5494,7 +5488,7 @@
         <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5899,7 +5893,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6113,7 +6107,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>31</v>
@@ -6151,7 +6145,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>32</v>
@@ -6194,28 +6188,166 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E266E0-7523-413E-8B0C-F3E2413808A5}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
     <col min="2" max="3" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>86</v>
+      <c r="A1" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8">
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <v>44671</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8">
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <v>44671.041666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <v>44671.08333321759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <v>44671.124999826388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <v>44671.166666435187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <v>44671.208333043978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <v>44671.249999537038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <v>44671.291666087964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <v>44671.333332638889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <v>44671.374999189815</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="str">
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="str">
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="str">
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="str">
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="str">
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="str">
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="str">
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="str">
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="str">
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="str">
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="str">
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="str">
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="str">
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="str">
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6248,7 +6380,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6436,7 +6568,7 @@
         <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>56</v>
@@ -6445,7 +6577,7 @@
         <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -6806,7 +6938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB98B755-8BE1-4837-9877-4DDB59C80C3F}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -6826,7 +6958,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6834,7 +6966,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6842,7 +6974,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6850,7 +6982,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6858,7 +6990,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6866,7 +6998,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7">
         <v>10000</v>
@@ -6874,7 +7006,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8">
         <v>10000</v>
@@ -6882,7 +7014,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6890,7 +7022,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -6977,7 +7109,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>0.3</v>
@@ -6993,7 +7125,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7590,13 +7722,13 @@
         <v>79</v>
       </c>
       <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
         <v>99</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>100</v>
-      </c>
-      <c r="J1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -8062,7 +8194,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
@@ -8077,13 +8209,13 @@
         <v>51</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>53</v>
@@ -8191,7 +8323,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
@@ -8384,7 +8516,7 @@
         <v>44</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>45</v>
@@ -8551,7 +8683,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="7">
         <v>0</v>
@@ -8604,7 +8736,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
@@ -8689,7 +8821,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -8700,7 +8832,7 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -8711,7 +8843,7 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -8719,10 +8851,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -8730,10 +8862,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -8847,10 +8979,10 @@
         <v>19</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -9047,7 +9179,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>21</v>
@@ -9079,13 +9211,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -9111,7 +9243,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>21</v>
@@ -9143,13 +9275,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -9363,19 +9495,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="C1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated example input data files with common_end parameters
Updated example input data files with common_end parameters in the "setup"-sheet.
</commit_message>
<xml_diff>
--- a/input_data/demo_model.xlsx
+++ b/input_data/demo_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896003F0-FF4F-4E26-A1DB-4BA8500D72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29F9F6-B68D-44BC-94AB-B3530B6CDFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="4" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
   <si>
     <t>node</t>
   </si>
@@ -401,9 +401,6 @@
     <t>use_ramp_dummy_variables</t>
   </si>
   <si>
-    <t>common_timesteps</t>
-  </si>
-  <si>
     <t>common_scenario_name</t>
   </si>
   <si>
@@ -435,6 +432,12 @@
   </si>
   <si>
     <t>group_type</t>
+  </si>
+  <si>
+    <t>common_start_timesteps</t>
+  </si>
+  <si>
+    <t>common_end_timesteps</t>
   </si>
 </sst>
 </file>
@@ -6159,7 +6162,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -6684,10 +6687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB98B755-8BE1-4837-9877-4DDB59C80C3F}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6746,7 +6749,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>10000</v>
@@ -6754,7 +6757,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>10000</v>
@@ -6762,7 +6765,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6770,7 +6773,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>125</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -8569,13 +8580,13 @@
         <v>49</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>107</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>51</v>
@@ -8876,7 +8887,7 @@
         <v>42</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>43</v>
@@ -9156,7 +9167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5539A729-4FB7-440D-A765-676495DE3453}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9164,7 +9175,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>60</v>
@@ -9330,7 +9341,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>20</v>
@@ -9339,10 +9350,10 @@
         <v>19</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>